<commit_message>
aggregate functions code from Wed.
</commit_message>
<xml_diff>
--- a/week12/day01/desigining database tables examples.xlsx
+++ b/week12/day01/desigining database tables examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehicks\SkillStorm\jon_javavettec20221003\100322-VET-TEC-Java\week12\day01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C107B42E-2136-40F9-8345-B4976BC7ED4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BFB3BB-44EA-417E-BCB9-25B601BAAF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF2F2CC-C33D-4AF8-A6BE-F4FAB35C5017}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDF2F2CC-C33D-4AF8-A6BE-F4FAB35C5017}"/>
   </bookViews>
   <sheets>
     <sheet name="Key Examples" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="115">
   <si>
     <t>Excel is NOT a databse, it is for visualizing data</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>item_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -1459,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984E9EF9-D4A6-40CF-BA88-2AF84A740959}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:G51"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2369,10 +2372,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6519FDBC-C4F3-4824-A13A-01546B269AA5}">
-  <dimension ref="A1:H122"/>
+  <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2380,7 +2383,7 @@
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2406,7 +2409,7 @@
       </c>
       <c r="B3" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="C3" t="s">
         <v>80</v>
@@ -2418,7 +2421,7 @@
       </c>
       <c r="B4" s="4">
         <f t="shared" ref="B4:B5" ca="1" si="0">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="C4" t="s">
         <v>82</v>
@@ -2430,7 +2433,7 @@
       </c>
       <c r="B5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="C5" t="s">
         <v>83</v>
@@ -2453,7 +2456,7 @@
       </c>
       <c r="B7" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="C7" t="s">
         <v>86</v>
@@ -2498,7 +2501,7 @@
       </c>
       <c r="C14" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D14" t="s">
         <v>80</v>
@@ -2513,7 +2516,7 @@
       </c>
       <c r="C15" s="4">
         <f t="shared" ref="C15:C16" ca="1" si="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D15" t="s">
         <v>82</v>
@@ -2528,13 +2531,13 @@
       </c>
       <c r="C16" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2548,7 +2551,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
@@ -2557,13 +2560,13 @@
       </c>
       <c r="C18" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -2577,12 +2580,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>88</v>
       </c>
@@ -2608,7 +2611,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2617,7 +2620,7 @@
       </c>
       <c r="C24" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D24" t="s">
         <v>103</v>
@@ -2628,8 +2631,11 @@
       <c r="F24" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2638,7 +2644,7 @@
       </c>
       <c r="C25" s="4">
         <f t="shared" ref="C25:C26" ca="1" si="2">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D25" t="s">
         <v>102</v>
@@ -2647,7 +2653,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2656,7 +2662,7 @@
       </c>
       <c r="C26" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D26" t="s">
         <v>104</v>
@@ -2665,7 +2671,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2679,7 +2685,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>5</v>
       </c>
@@ -2688,7 +2694,7 @@
       </c>
       <c r="C28" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D28" t="s">
         <v>92</v>
@@ -2700,7 +2706,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2714,7 +2720,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>90</v>
       </c>
@@ -2742,7 +2748,7 @@
       </c>
       <c r="C34" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D34" t="s">
         <v>103</v>
@@ -2757,7 +2763,7 @@
       </c>
       <c r="C35" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D35" t="s">
         <v>98</v>
@@ -2772,7 +2778,7 @@
       </c>
       <c r="C36" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D36" t="s">
         <v>99</v>
@@ -2787,7 +2793,7 @@
       </c>
       <c r="C37" s="4">
         <f t="shared" ref="C37:C39" ca="1" si="3">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D37" t="s">
         <v>102</v>
@@ -2802,7 +2808,7 @@
       </c>
       <c r="C38" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D38" t="s">
         <v>100</v>
@@ -2817,7 +2823,7 @@
       </c>
       <c r="C39" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D39" t="s">
         <v>104</v>
@@ -2832,7 +2838,7 @@
       </c>
       <c r="C40" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D40" t="s">
         <v>105</v>
@@ -2861,7 +2867,7 @@
       </c>
       <c r="C42" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D42" t="s">
         <v>106</v>
@@ -2876,7 +2882,7 @@
       </c>
       <c r="C43" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D43" t="s">
         <v>101</v>
@@ -2891,7 +2897,7 @@
       </c>
       <c r="C44" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
       <c r="D44" t="s">
         <v>92</v>
@@ -2936,7 +2942,7 @@
       </c>
       <c r="C50" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2948,7 +2954,7 @@
       </c>
       <c r="C51" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2960,7 +2966,7 @@
       </c>
       <c r="C52" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2983,7 +2989,7 @@
       </c>
       <c r="C54" s="4">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -3158,7 +3164,7 @@
       </c>
       <c r="C80" s="9">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -3170,7 +3176,7 @@
       </c>
       <c r="C81" s="9">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -3182,7 +3188,7 @@
       </c>
       <c r="C82" s="9">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -3205,7 +3211,7 @@
       </c>
       <c r="C84" s="9">
         <f ca="1">TODAY()</f>
-        <v>44915</v>
+        <v>44917</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>